<commit_message>
add in color family selections
</commit_message>
<xml_diff>
--- a/data/DMC_Embroidery_Floss_Color_Families_2021.xlsx
+++ b/data/DMC_Embroidery_Floss_Color_Families_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurahughes/GitHub/image2dmc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A22E6F-5580-6449-9D19-C5C83EF9C1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBEC911-3DE1-B248-9362-3E4C1043F649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="660" windowWidth="13140" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34740" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -4987,9 +4987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M483"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="19"/>
@@ -5076,7 +5076,7 @@
         <v>542</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20">
@@ -5099,7 +5099,7 @@
         <v>542</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="20">
@@ -5122,7 +5122,7 @@
         <v>542</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20">
@@ -5145,7 +5145,7 @@
         <v>542</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20">
@@ -5168,7 +5168,7 @@
         <v>542</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20">
@@ -5191,7 +5191,7 @@
         <v>542</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20">
@@ -5214,7 +5214,7 @@
         <v>542</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="20">
@@ -5237,7 +5237,7 @@
         <v>542</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="20">
@@ -5260,7 +5260,7 @@
         <v>542</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="20">
@@ -5283,7 +5283,7 @@
         <v>542</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="20">
@@ -5306,7 +5306,7 @@
         <v>542</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="20">
@@ -5329,7 +5329,7 @@
         <v>542</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="20">
@@ -5352,7 +5352,7 @@
         <v>542</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20">
@@ -5375,7 +5375,7 @@
         <v>542</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="20">
@@ -5398,7 +5398,7 @@
         <v>542</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20">
@@ -5421,7 +5421,7 @@
         <v>542</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20">
@@ -5444,7 +5444,7 @@
         <v>542</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20">
@@ -5479,7 +5479,7 @@
         <v>542</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20">
@@ -5502,7 +5502,7 @@
         <v>542</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20">
@@ -5525,7 +5525,7 @@
         <v>542</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20">
@@ -5548,7 +5548,7 @@
         <v>542</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20">
@@ -5571,7 +5571,7 @@
         <v>542</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20">
@@ -5594,7 +5594,7 @@
         <v>542</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20">
@@ -5617,7 +5617,7 @@
         <v>542</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20">
@@ -16237,7 +16237,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J483">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K483">
     <sortCondition ref="J2:J483"/>
     <sortCondition ref="I2:I483"/>
   </sortState>

</xml_diff>